<commit_message>
updated oly sampling spreadsheet with K data
</commit_message>
<xml_diff>
--- a/Data/2017-02-04_SamplingData.xlsx
+++ b/Data/2017-02-04_SamplingData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="0" windowWidth="24100" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="580" yWindow="0" windowWidth="24100" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,9 +417,6 @@
     <t>HL-10 (warm overwinter temp)</t>
   </si>
   <si>
-    <t>Not sampled</t>
-  </si>
-  <si>
     <t>Sampling Date</t>
   </si>
   <si>
@@ -427,6 +424,9 @@
   </si>
   <si>
     <t>Sampled Tissue in Ethanol: Misc tissue (mix of M,C or A);</t>
+  </si>
+  <si>
+    <t># on K-Ethanol DNA Tube</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -547,8 +547,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -560,8 +562,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -583,6 +596,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -604,6 +618,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -936,7 +951,8 @@
   <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <pane ySplit="4" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -945,7 +961,7 @@
     <col min="3" max="3" width="14.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="33" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" style="9" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="54.33203125" style="3" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="3"/>
@@ -953,25 +969,28 @@
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
-        <v>133</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
       <c r="A2" s="6" t="s">
-        <v>134</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="51" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>110</v>
@@ -993,7 +1012,7 @@
       <c r="E5" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
@@ -1002,13 +1021,13 @@
       <c r="B6" s="4">
         <v>42770</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="10">
         <v>31.1</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="10">
         <v>6.3</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
@@ -1017,13 +1036,13 @@
       <c r="B7" s="4">
         <v>42770</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="10">
         <v>33.9</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="10">
         <v>7.8</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
@@ -1032,13 +1051,13 @@
       <c r="B8" s="4">
         <v>42770</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="10">
         <v>37.4</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="10">
         <v>11</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
@@ -1047,13 +1066,13 @@
       <c r="B9" s="4">
         <v>42770</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="10">
         <v>33.1</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="10">
         <v>8.6</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
@@ -1062,13 +1081,13 @@
       <c r="B10" s="4">
         <v>42770</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="10">
         <v>35</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="10">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
@@ -1077,13 +1096,13 @@
       <c r="B11" s="4">
         <v>42770</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="10">
         <v>31.2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="10">
         <v>7.2</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
@@ -1092,13 +1111,13 @@
       <c r="B12" s="4">
         <v>42770</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="10">
         <v>31.9</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="10">
         <v>5.4</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
@@ -1107,13 +1126,13 @@
       <c r="B13" s="4">
         <v>42770</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="10">
         <v>30.4</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="10">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
@@ -1122,16 +1141,16 @@
       <c r="B14" s="4">
         <v>42770</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="10">
         <v>40.4</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="10">
         <v>10.8</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
@@ -1140,13 +1159,13 @@
       <c r="B15" s="4">
         <v>42770</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="10">
         <v>34.299999999999997</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="10">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
@@ -1155,16 +1174,16 @@
       <c r="B16" s="4">
         <v>42770</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="10">
         <v>31.1</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="10">
         <v>7.3</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
@@ -1173,13 +1192,13 @@
       <c r="B17" s="4">
         <v>42770</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="10">
         <v>29.2</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="10">
         <v>5.3</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
@@ -1188,13 +1207,13 @@
       <c r="B18" s="4">
         <v>42770</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="10">
         <v>33.299999999999997</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="10">
         <v>6.3</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
@@ -1203,13 +1222,13 @@
       <c r="B19" s="4">
         <v>42770</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="10">
         <v>26.5</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="10">
         <v>4.5</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
@@ -1218,32 +1237,32 @@
       <c r="B20" s="4">
         <v>42770</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="10">
         <v>27.1</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="10">
         <v>4.7</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
@@ -1252,13 +1271,13 @@
       <c r="B23" s="4">
         <v>42770</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="10">
         <v>27.9</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="10">
         <v>6.4</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
@@ -1267,13 +1286,13 @@
       <c r="B24" s="4">
         <v>42770</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="10">
         <v>30.5</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="10">
         <v>6</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
@@ -1282,16 +1301,16 @@
       <c r="B25" s="4">
         <v>42770</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="10">
         <v>38.1</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="10">
         <v>9.1</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
@@ -1300,13 +1319,13 @@
       <c r="B26" s="4">
         <v>42770</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="10">
         <v>37.5</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="10">
         <v>11.1</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
@@ -1315,13 +1334,13 @@
       <c r="B27" s="4">
         <v>42770</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="10">
         <v>34.4</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="10">
         <v>8.1</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
@@ -1330,13 +1349,13 @@
       <c r="B28" s="4">
         <v>42770</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="10">
         <v>34.799999999999997</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="10">
         <v>10</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
@@ -1345,13 +1364,13 @@
       <c r="B29" s="4">
         <v>42770</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="10">
         <v>36</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="10">
         <v>10.6</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
@@ -1360,13 +1379,13 @@
       <c r="B30" s="4">
         <v>42770</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="10">
         <v>40.4</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="10">
         <v>10.7</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
@@ -1375,13 +1394,13 @@
       <c r="B31" s="4">
         <v>42770</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="10">
         <v>37.4</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="10">
         <v>7.9</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
@@ -1390,13 +1409,13 @@
       <c r="B32" s="4">
         <v>42770</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="10">
         <v>26.5</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="10">
         <v>7.1</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
@@ -1405,13 +1424,13 @@
       <c r="B33" s="4">
         <v>42770</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="10">
         <v>39.9</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="10">
         <v>5.9</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
@@ -1420,16 +1439,16 @@
       <c r="B34" s="4">
         <v>42770</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="10">
         <v>30.5</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="10">
         <v>7.2</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
@@ -1438,13 +1457,13 @@
       <c r="B35" s="4">
         <v>42770</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="10">
         <v>31.4</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="10">
         <v>7</v>
       </c>
-      <c r="F35" s="2"/>
+      <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
@@ -1453,13 +1472,13 @@
       <c r="B36" s="4">
         <v>42770</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="10">
         <v>26.5</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="10">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
@@ -1468,18 +1487,24 @@
       <c r="B37" s="4">
         <v>42770</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="10">
         <v>26.5</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="10">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="3" t="s">
         <v>118</v>
       </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
       <c r="E39" s="3" t="s">
         <v>119</v>
       </c>
@@ -1491,13 +1516,13 @@
       <c r="B40" s="4">
         <v>42770</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="10">
         <v>29.1</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="10">
         <v>4.7</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
@@ -1506,13 +1531,13 @@
       <c r="B41" s="4">
         <v>42770</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="10">
         <v>36.1</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="10">
         <v>7.6</v>
       </c>
-      <c r="F41" s="2"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
@@ -1521,13 +1546,13 @@
       <c r="B42" s="4">
         <v>42770</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="10">
         <v>27.5</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="10">
         <v>5.3</v>
       </c>
-      <c r="F42" s="2"/>
+      <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
@@ -1536,13 +1561,13 @@
       <c r="B43" s="4">
         <v>42770</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="10">
         <v>38.5</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="10">
         <v>7.1</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
@@ -1551,13 +1576,13 @@
       <c r="B44" s="4">
         <v>42770</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="10">
         <v>34.1</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="10">
         <v>7.8</v>
       </c>
-      <c r="F44" s="2"/>
+      <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
@@ -1566,13 +1591,13 @@
       <c r="B45" s="4">
         <v>42770</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="10">
         <v>39.6</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="10">
         <v>7.1</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
@@ -1581,13 +1606,13 @@
       <c r="B46" s="4">
         <v>42770</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="10">
         <v>29</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="10">
         <v>5.6</v>
       </c>
-      <c r="F46" s="2"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
@@ -1596,13 +1621,13 @@
       <c r="B47" s="4">
         <v>42770</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="10">
         <v>38.4</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="10">
         <v>10.4</v>
       </c>
-      <c r="F47" s="2"/>
+      <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
@@ -1611,16 +1636,16 @@
       <c r="B48" s="4">
         <v>42770</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="10">
         <v>38.4</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="10">
         <v>7.6</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F48" s="2"/>
+      <c r="F48" s="8"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
@@ -1629,13 +1654,13 @@
       <c r="B49" s="4">
         <v>42770</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="10">
         <v>25.1</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="10">
         <v>2.9</v>
       </c>
-      <c r="F49" s="2"/>
+      <c r="F49" s="8"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
@@ -1644,13 +1669,13 @@
       <c r="B50" s="4">
         <v>42770</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="10">
         <v>36.5</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="10">
         <v>8.5</v>
       </c>
-      <c r="F50" s="2"/>
+      <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
@@ -1659,13 +1684,13 @@
       <c r="B51" s="4">
         <v>42770</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="10">
         <v>24.5</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="10">
         <v>3.3</v>
       </c>
-      <c r="F51" s="2"/>
+      <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
@@ -1674,13 +1699,13 @@
       <c r="B52" s="4">
         <v>42770</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="10">
         <v>37.4</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="10">
         <v>8.4</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="8"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
@@ -1689,13 +1714,13 @@
       <c r="B53" s="4">
         <v>42770</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="10">
         <v>40.020000000000003</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="10">
         <v>9.1</v>
       </c>
-      <c r="F53" s="2"/>
+      <c r="F53" s="8"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
@@ -1704,18 +1729,24 @@
       <c r="B54" s="4">
         <v>42770</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="10">
         <v>28.4</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="10">
         <v>5.9</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="3" t="s">
         <v>121</v>
       </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
       <c r="E56" s="3" t="s">
         <v>122</v>
       </c>
@@ -1727,13 +1758,13 @@
       <c r="B57" s="4">
         <v>42770</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="10">
         <v>30.56</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="10">
         <v>5.7</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="8"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
@@ -1742,13 +1773,13 @@
       <c r="B58" s="4">
         <v>42770</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="10">
         <v>33.5</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="10">
         <v>8.4</v>
       </c>
-      <c r="F58" s="2"/>
+      <c r="F58" s="8"/>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2" t="s">
@@ -1757,13 +1788,13 @@
       <c r="B59" s="4">
         <v>42770</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="10">
         <v>25.6</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="10">
         <v>3.5</v>
       </c>
-      <c r="F59" s="2"/>
+      <c r="F59" s="8"/>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
@@ -1772,16 +1803,16 @@
       <c r="B60" s="4">
         <v>42770</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="10">
         <v>33.4</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="10">
         <v>8.6</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F60" s="2"/>
+      <c r="F60" s="8"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
@@ -1790,16 +1821,16 @@
       <c r="B61" s="4">
         <v>42770</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="10">
         <v>36.4</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="10">
         <v>9.5</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F61" s="2"/>
+      <c r="F61" s="8"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
@@ -1808,16 +1839,16 @@
       <c r="B62" s="4">
         <v>42770</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="10">
         <v>35.5</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="10">
         <v>8.6</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F62" s="2"/>
+      <c r="F62" s="8"/>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
@@ -1826,16 +1857,16 @@
       <c r="B63" s="4">
         <v>42770</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="10">
         <v>42.2</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="10">
         <v>8.6999999999999993</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F63" s="2"/>
+      <c r="F63" s="8"/>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
@@ -1844,16 +1875,16 @@
       <c r="B64" s="4">
         <v>42770</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="10">
         <v>22</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="10">
         <v>3.4</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F64" s="2"/>
+      <c r="F64" s="8"/>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
@@ -1862,16 +1893,16 @@
       <c r="B65" s="4">
         <v>42770</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="10">
         <v>35.299999999999997</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="10">
         <v>5.2</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="F65" s="2"/>
+      <c r="F65" s="8"/>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
@@ -1880,13 +1911,13 @@
       <c r="B66" s="4">
         <v>42770</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="10">
         <v>34.1</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="10">
         <v>5.6</v>
       </c>
-      <c r="F66" s="2"/>
+      <c r="F66" s="8"/>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
@@ -1895,13 +1926,13 @@
       <c r="B67" s="4">
         <v>42770</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="10">
         <v>25.4</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="10">
         <v>4.2</v>
       </c>
-      <c r="F67" s="2"/>
+      <c r="F67" s="8"/>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
@@ -1910,16 +1941,16 @@
       <c r="B68" s="4">
         <v>42770</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="10">
         <v>30.5</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="10">
         <v>9.4</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F68" s="2"/>
+      <c r="F68" s="8"/>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
@@ -1928,13 +1959,13 @@
       <c r="B69" s="4">
         <v>42770</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="10">
         <v>37.119999999999997</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="10">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F69" s="2"/>
+      <c r="F69" s="8"/>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
@@ -1943,13 +1974,13 @@
       <c r="B70" s="4">
         <v>42770</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="10">
         <v>37.1</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70" s="10">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F70" s="2"/>
+      <c r="F70" s="8"/>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2" t="s">
@@ -1958,17 +1989,23 @@
       <c r="B71" s="4">
         <v>42770</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="10">
         <v>29</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="10">
         <v>5.4</v>
       </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="3" t="s">
         <v>129</v>
       </c>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
       <c r="E73" s="3" t="s">
         <v>116</v>
       </c>
@@ -1980,10 +2017,10 @@
       <c r="B74" s="4">
         <v>42770</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="10">
         <v>26.1</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74" s="10">
         <v>6.7</v>
       </c>
       <c r="E74" s="3" t="s">
@@ -1997,10 +2034,10 @@
       <c r="B75" s="4">
         <v>42770</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="10">
         <v>21.7</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75" s="10">
         <v>2</v>
       </c>
       <c r="E75" s="3" t="s">
@@ -2014,10 +2051,10 @@
       <c r="B76" s="4">
         <v>42770</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="10">
         <v>20.3</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D76" s="10">
         <v>2.6</v>
       </c>
     </row>
@@ -2028,10 +2065,10 @@
       <c r="B77" s="4">
         <v>42770</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="10">
         <v>25.6</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77" s="10">
         <v>3.2</v>
       </c>
     </row>
@@ -2042,10 +2079,10 @@
       <c r="B78" s="4">
         <v>42770</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="10">
         <v>30.4</v>
       </c>
-      <c r="D78" s="2">
+      <c r="D78" s="10">
         <v>4.3</v>
       </c>
     </row>
@@ -2056,10 +2093,10 @@
       <c r="B79" s="4">
         <v>42770</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="10">
         <v>36.5</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D79" s="10">
         <v>8.6</v>
       </c>
     </row>
@@ -2070,416 +2107,701 @@
       <c r="B80" s="4">
         <v>42770</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="10">
         <v>28.9</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80" s="10">
         <v>4.7</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B81" s="4">
         <v>42770</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="10">
         <v>29.5</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81" s="10">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:6">
       <c r="A82" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B82" s="4">
         <v>42770</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="10">
         <v>35</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D82" s="10">
         <v>6.9</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="83" spans="1:6">
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="3" t="s">
         <v>130</v>
       </c>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
       <c r="E84" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:6">
       <c r="A85" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B85" s="4">
         <v>42770</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85" s="10">
         <v>27</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D85" s="10">
         <v>5.8</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:6">
       <c r="A86" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B86" s="4">
         <v>42770</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="10">
         <v>24.2</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86" s="10">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:6">
       <c r="A87" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B87" s="4">
         <v>42770</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="10">
         <v>30.5</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D87" s="10">
         <v>5.8</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:6">
       <c r="A88" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B88" s="4">
         <v>42770</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88" s="10">
         <v>34.9</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88" s="10">
         <v>8.5</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:6">
       <c r="A89" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B89" s="4">
         <v>42770</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="10">
         <v>32</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D89" s="10">
         <v>5.8</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:6">
       <c r="A90" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B90" s="4">
         <v>42770</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90" s="10">
         <v>28</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="10">
         <v>3.9</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:6">
       <c r="A91" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B91" s="4">
         <v>42770</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C91" s="10">
         <v>34.700000000000003</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="10">
         <v>6.6</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:6">
       <c r="A92" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B92" s="4">
         <v>42770</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C92" s="10">
         <v>34.1</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92" s="10">
         <v>7.2</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:6">
       <c r="A93" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B93" s="4">
         <v>42770</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93" s="10">
         <v>31</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93" s="10">
         <v>5.5</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="94" spans="1:6">
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="B95" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C95" s="10">
+        <v>20.02</v>
+      </c>
+      <c r="D95" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="F95" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="B96" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C96" s="10">
+        <v>29.5</v>
+      </c>
+      <c r="D96" s="10">
+        <v>2.8</v>
+      </c>
+      <c r="F96" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="B97" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C97" s="10">
+        <v>18.3</v>
+      </c>
+      <c r="D97" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="F97" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="B98" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C98" s="10">
+        <v>21.2</v>
+      </c>
+      <c r="D98" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="F98" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="B99" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C99" s="10">
+        <v>24.3</v>
+      </c>
+      <c r="D99" s="10">
+        <v>2.6</v>
+      </c>
+      <c r="F99" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="B100" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C100" s="10">
+        <v>28.3</v>
+      </c>
+      <c r="D100" s="10">
+        <v>2.7</v>
+      </c>
+      <c r="F100" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="B101" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C101" s="10">
+        <v>20.04</v>
+      </c>
+      <c r="D101" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="F101" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="B102" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C102" s="10">
+        <v>20.059999999999999</v>
+      </c>
+      <c r="D102" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F102" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="B103" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C103" s="10">
+        <v>16.8</v>
+      </c>
+      <c r="D103" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="F103" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="B104" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C104" s="10">
+        <v>21.8</v>
+      </c>
+      <c r="D104" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="F104" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="B105" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C105" s="10">
+        <v>23.7</v>
+      </c>
+      <c r="D105" s="10">
+        <v>1.9</v>
+      </c>
+      <c r="F105" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="B106" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C106" s="10">
+        <v>27.5</v>
+      </c>
+      <c r="D106" s="10">
+        <v>3</v>
+      </c>
+      <c r="F106" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="B107" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C107" s="10">
+        <v>21.6</v>
+      </c>
+      <c r="D107" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="F107" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="B108" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C108" s="10">
+        <v>24.1</v>
+      </c>
+      <c r="D108" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="F108" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="B109" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C109" s="10">
+        <v>22.5</v>
+      </c>
+      <c r="D109" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="F109" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="F110" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D111" s="2"/>
-    </row>
-    <row r="112" spans="1:4">
+      <c r="B111" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C111" s="10">
+        <v>23.8</v>
+      </c>
+      <c r="D111" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="F111" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="B112" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C112" s="10">
+        <v>21.5</v>
+      </c>
+      <c r="D112" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="F112" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="B113" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C113" s="10">
+        <v>24.6</v>
+      </c>
+      <c r="D113" s="10">
+        <v>2.6</v>
+      </c>
+      <c r="F113" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="2"/>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="B114" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C114" s="10">
+        <v>17.7</v>
+      </c>
+      <c r="D114" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="F114" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="B115" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C115" s="10">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="D115" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="F115" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="B116" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C116" s="10">
+        <v>19.5</v>
+      </c>
+      <c r="D116" s="10">
+        <v>1</v>
+      </c>
+      <c r="F116" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="B117" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C117" s="10">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="D117" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="F117" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="B118" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C118" s="10">
+        <v>19.5</v>
+      </c>
+      <c r="D118" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="F118" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="B119" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C119" s="10">
+        <v>21.5</v>
+      </c>
+      <c r="D119" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="F119" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="B120" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C120" s="10">
+        <v>22.5</v>
+      </c>
+      <c r="D120" s="10">
+        <v>1.9</v>
+      </c>
+      <c r="F120" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="B121" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C121" s="10">
+        <v>18.7</v>
+      </c>
+      <c r="D121" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="F121" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="B122" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C122" s="10">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D122" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="F122" s="9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="B123" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C123" s="10">
+        <v>26.5</v>
+      </c>
+      <c r="D123" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F123" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="B124" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C124" s="10">
+        <v>25</v>
+      </c>
+      <c r="D124" s="10">
+        <v>1.9</v>
+      </c>
+      <c r="F124" s="9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
+      <c r="B125" s="4">
+        <v>42777</v>
+      </c>
+      <c r="C125" s="10">
+        <v>21.3</v>
+      </c>
+      <c r="D125" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="F125" s="9">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
updated lots of things
</commit_message>
<xml_diff>
--- a/Data/2017-02-04_SamplingData.xlsx
+++ b/Data/2017-02-04_SamplingData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="0" windowWidth="24100" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="15260" yWindow="0" windowWidth="11200" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -951,8 +951,8 @@
   <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
uploaded images of oly spawning setup
</commit_message>
<xml_diff>
--- a/Data/2017-02-04_SamplingData.xlsx
+++ b/Data/2017-02-04_SamplingData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15260" yWindow="0" windowWidth="11200" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="8220" yWindow="0" windowWidth="17280" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="149">
   <si>
     <t>Oyster #</t>
   </si>
@@ -378,18 +378,12 @@
     <t>Very ripe</t>
   </si>
   <si>
-    <t>NF-6 (cold overwinter temp)</t>
-  </si>
-  <si>
     <t>2 morts</t>
   </si>
   <si>
     <t>Appeared emaciated</t>
   </si>
   <si>
-    <t>NF010 (warm overwintering temp)</t>
-  </si>
-  <si>
     <t>1 mort</t>
   </si>
   <si>
@@ -427,6 +421,54 @@
   </si>
   <si>
     <t># on K-Ethanol DNA Tube</t>
+  </si>
+  <si>
+    <t>Gonad Stage (ID'd from slides)</t>
+  </si>
+  <si>
+    <t>Notes on Histology Image</t>
+  </si>
+  <si>
+    <t>Early Male</t>
+  </si>
+  <si>
+    <t>Loose spermatocyte balls forming, no oocytes visible, lots of empty connective tissue</t>
+  </si>
+  <si>
+    <t>Plckets of loose spermatocyte balls forming, spermatogonia loosely present, no oocytes visible, lots of empty connective tissue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undeveloped, Indeterminate  </t>
+  </si>
+  <si>
+    <t>NF010 (ambient)</t>
+  </si>
+  <si>
+    <t>NF-6 (chilled)</t>
+  </si>
+  <si>
+    <t>Mostly empty connective tissue; some remnant spermatocytes, a few degraded oocytes, some spermatogonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pockets of loose spermatocytes (not distinct balls); no oocytes present (possibly a few degraded); </t>
+  </si>
+  <si>
+    <t>Early/Mid(?) Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid, Indeterminate </t>
+  </si>
+  <si>
+    <t>Possibly resorbing oocytes?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possibly resorbing? Looks like mature oocytes present, lots of empty connective tissue, and </t>
+  </si>
+  <si>
+    <t>Late Female</t>
+  </si>
+  <si>
+    <t>Undeveloped Male</t>
   </si>
 </sst>
 </file>
@@ -503,7 +545,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -549,8 +591,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -573,8 +621,11 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -597,6 +648,9 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -619,6 +673,9 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -948,49 +1005,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <pane ySplit="4" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="11.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="3" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="3" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="3" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="29.83203125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="28" style="3" customWidth="1"/>
     <col min="8" max="8" width="54.33203125" style="3" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1">
+    <row r="1" spans="1:7" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1">
+    <row r="2" spans="1:7" s="6" customFormat="1">
       <c r="A2" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" s="6" customFormat="1">
+    <row r="3" spans="1:7" s="6" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="51" customHeight="1">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="51" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>110</v>
@@ -1001,8 +1059,14 @@
       <c r="E4" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>115</v>
       </c>
@@ -1014,7 +1078,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1029,7 +1093,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1044,7 +1108,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1059,7 +1123,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -1074,7 +1138,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1089,7 +1153,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1104,7 +1168,7 @@
       </c>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1119,7 +1183,7 @@
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1134,7 +1198,7 @@
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1152,7 +1216,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -1167,7 +1231,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1260,7 +1324,7 @@
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -1417,7 +1481,7 @@
       </c>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
@@ -1432,7 +1496,7 @@
       </c>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1450,7 +1514,7 @@
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:7">
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
@@ -1465,7 +1529,7 @@
       </c>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:7">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
@@ -1480,7 +1544,7 @@
       </c>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:7">
       <c r="A37" s="2" t="s">
         <v>47</v>
       </c>
@@ -1495,21 +1559,21 @@
       </c>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:7">
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:7">
       <c r="A39" s="3" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="2" t="s">
         <v>16</v>
       </c>
@@ -1522,9 +1586,14 @@
       <c r="D40" s="10">
         <v>4.7</v>
       </c>
-      <c r="F40" s="8"/>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="F40" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="2" t="s">
         <v>17</v>
       </c>
@@ -1537,9 +1606,14 @@
       <c r="D41" s="10">
         <v>7.6</v>
       </c>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="F41" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -1552,9 +1626,14 @@
       <c r="D42" s="10">
         <v>5.3</v>
       </c>
-      <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="F42" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -1567,9 +1646,14 @@
       <c r="D43" s="10">
         <v>7.1</v>
       </c>
-      <c r="F43" s="8"/>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="F43" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="2" t="s">
         <v>20</v>
       </c>
@@ -1582,9 +1666,14 @@
       <c r="D44" s="10">
         <v>7.8</v>
       </c>
-      <c r="F44" s="8"/>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="F44" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
@@ -1597,9 +1686,14 @@
       <c r="D45" s="10">
         <v>7.1</v>
       </c>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="F45" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
@@ -1612,9 +1706,11 @@
       <c r="D46" s="10">
         <v>5.6</v>
       </c>
-      <c r="F46" s="8"/>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="F46" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
@@ -1629,7 +1725,7 @@
       </c>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:7">
       <c r="A48" s="2" t="s">
         <v>24</v>
       </c>
@@ -1643,7 +1739,7 @@
         <v>7.6</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F48" s="8"/>
     </row>
@@ -1743,12 +1839,12 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="3" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
       <c r="E56" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1810,7 +1906,7 @@
         <v>8.6</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F60" s="8"/>
     </row>
@@ -1828,7 +1924,7 @@
         <v>9.5</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F61" s="8"/>
     </row>
@@ -1846,7 +1942,7 @@
         <v>8.6</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F62" s="8"/>
     </row>
@@ -1900,7 +1996,7 @@
         <v>5.2</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F65" s="8"/>
     </row>
@@ -1948,7 +2044,7 @@
         <v>9.4</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F68" s="8"/>
     </row>
@@ -2002,7 +2098,7 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
@@ -2024,7 +2120,7 @@
         <v>6.7</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2041,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2148,7 +2244,7 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
@@ -2545,7 +2641,7 @@
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
       <c r="F110" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="111" spans="1:6">

</xml_diff>

<commit_message>
Updated sampling and larval collection data
</commit_message>
<xml_diff>
--- a/Data/2017-02-04_SamplingData.xlsx
+++ b/Data/2017-02-04_SamplingData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="0" windowWidth="17280" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="25460" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="149">
   <si>
     <t>Oyster #</t>
   </si>
@@ -423,39 +423,12 @@
     <t># on K-Ethanol DNA Tube</t>
   </si>
   <si>
-    <t>Gonad Stage (ID'd from slides)</t>
-  </si>
-  <si>
-    <t>Notes on Histology Image</t>
-  </si>
-  <si>
-    <t>Early Male</t>
-  </si>
-  <si>
-    <t>Loose spermatocyte balls forming, no oocytes visible, lots of empty connective tissue</t>
-  </si>
-  <si>
-    <t>Plckets of loose spermatocyte balls forming, spermatogonia loosely present, no oocytes visible, lots of empty connective tissue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Undeveloped, Indeterminate  </t>
-  </si>
-  <si>
     <t>NF010 (ambient)</t>
   </si>
   <si>
     <t>NF-6 (chilled)</t>
   </si>
   <si>
-    <t>Mostly empty connective tissue; some remnant spermatocytes, a few degraded oocytes, some spermatogonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pockets of loose spermatocytes (not distinct balls); no oocytes present (possibly a few degraded); </t>
-  </si>
-  <si>
-    <t>Early/Mid(?) Male</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mid, Indeterminate </t>
   </si>
   <si>
@@ -468,14 +441,41 @@
     <t>Late Female</t>
   </si>
   <si>
-    <t>Undeveloped Male</t>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male </t>
+  </si>
+  <si>
+    <t>Ripeness Rating (1-3)</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some spermatozoa (sperm balls), lots of loose spermatids. Sperm in gonad canals?  </t>
+  </si>
+  <si>
+    <t>Empty connective tissue; Lots of remnant spermatocytes, a few degraded oocytes, some spermatogonia</t>
+  </si>
+  <si>
+    <t>Male / Ind.</t>
+  </si>
+  <si>
+    <t>Empty connective tissue; some spermatocytes and spermatids.</t>
+  </si>
+  <si>
+    <t>Strip of dense spermatids (unorganized, not in balls); some spermatocytes; lots of empty connective tissue in other areas of sample</t>
+  </si>
+  <si>
+    <t>Needs additional reviewing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -527,6 +527,22 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -545,7 +561,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -597,8 +613,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -610,22 +632,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -651,6 +675,9 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -676,6 +703,9 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1005,45 +1035,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+      <pane ySplit="4" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" activeCellId="4" sqref="D6:D20 D23:D37 D40:D50 D51:D54 D57:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="29.83203125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.33203125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="13" customWidth="1"/>
+    <col min="8" max="8" width="54.33203125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="50.83203125" style="13" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1">
+    <row r="1" spans="1:9" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" s="6" customFormat="1">
+      <c r="F1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" s="6" customFormat="1">
       <c r="A2" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" s="6" customFormat="1">
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" s="6" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="51" customHeight="1">
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="51" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1059,14 +1099,18 @@
       <c r="E4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>115</v>
       </c>
@@ -1076,178 +1120,178 @@
       <c r="E5" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="4">
         <v>42770</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>31.1</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>6.3</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4">
         <v>42770</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>33.9</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>7.8</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="4">
         <v>42770</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>37.4</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>11</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="4">
         <v>42770</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>33.1</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>8.6</v>
       </c>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4">
         <v>42770</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>35</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="4">
         <v>42770</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>31.2</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>7.2</v>
       </c>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="4">
         <v>42770</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>31.9</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>5.4</v>
       </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="4">
         <v>42770</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>30.4</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="4">
         <v>42770</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="7">
         <v>40.4</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="7">
         <v>10.8</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="4">
         <v>42770</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>34.299999999999997</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="7">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="4">
         <v>42770</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <v>31.1</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="7">
         <v>7.3</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
@@ -1256,13 +1300,13 @@
       <c r="B17" s="4">
         <v>42770</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="7">
         <v>29.2</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="7">
         <v>5.3</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
@@ -1271,13 +1315,13 @@
       <c r="B18" s="4">
         <v>42770</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <v>33.299999999999997</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="7">
         <v>6.3</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
@@ -1286,13 +1330,13 @@
       <c r="B19" s="4">
         <v>42770</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="7">
         <v>26.5</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="7">
         <v>4.5</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
@@ -1301,32 +1345,32 @@
       <c r="B20" s="4">
         <v>42770</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="7">
         <v>27.1</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="7">
         <v>4.7</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="F21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
@@ -1335,13 +1379,13 @@
       <c r="B23" s="4">
         <v>42770</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="7">
         <v>27.9</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="7">
         <v>6.4</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
@@ -1350,13 +1394,13 @@
       <c r="B24" s="4">
         <v>42770</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="7">
         <v>30.5</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="7">
         <v>6</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
@@ -1365,16 +1409,16 @@
       <c r="B25" s="4">
         <v>42770</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="7">
         <v>38.1</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="7">
         <v>9.1</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="8"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
@@ -1383,13 +1427,13 @@
       <c r="B26" s="4">
         <v>42770</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="7">
         <v>37.5</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="7">
         <v>11.1</v>
       </c>
-      <c r="F26" s="8"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
@@ -1398,13 +1442,13 @@
       <c r="B27" s="4">
         <v>42770</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="7">
         <v>34.4</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="7">
         <v>8.1</v>
       </c>
-      <c r="F27" s="8"/>
+      <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
@@ -1413,13 +1457,13 @@
       <c r="B28" s="4">
         <v>42770</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="7">
         <v>34.799999999999997</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="7">
         <v>10</v>
       </c>
-      <c r="F28" s="8"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
@@ -1428,13 +1472,13 @@
       <c r="B29" s="4">
         <v>42770</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="7">
         <v>36</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="7">
         <v>10.6</v>
       </c>
-      <c r="F29" s="8"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
@@ -1443,13 +1487,13 @@
       <c r="B30" s="4">
         <v>42770</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="7">
         <v>40.4</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="7">
         <v>10.7</v>
       </c>
-      <c r="F30" s="8"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
@@ -1458,13 +1502,13 @@
       <c r="B31" s="4">
         <v>42770</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="7">
         <v>37.4</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="7">
         <v>7.9</v>
       </c>
-      <c r="F31" s="8"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
@@ -1473,275 +1517,304 @@
       <c r="B32" s="4">
         <v>42770</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="7">
         <v>26.5</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="7">
         <v>7.1</v>
       </c>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B33" s="4">
         <v>42770</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="7">
         <v>39.9</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="7">
         <v>5.9</v>
       </c>
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B34" s="4">
         <v>42770</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="7">
         <v>30.5</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="7">
         <v>7.2</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="F34" s="12"/>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B35" s="4">
         <v>42770</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="7">
         <v>31.4</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="7">
         <v>7</v>
       </c>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="4">
         <v>42770</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="7">
         <v>26.5</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="7">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="4">
         <v>42770</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="7">
         <v>26.5</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
+        <v>134</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
       <c r="E39" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:9">
       <c r="A40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="4">
         <v>42770</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="7">
         <v>29.1</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="7">
         <v>4.7</v>
       </c>
-      <c r="F40" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="F40" s="14">
+        <v>2</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B41" s="4">
         <v>42770</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="7">
         <v>36.1</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="7">
         <v>7.6</v>
       </c>
-      <c r="F41" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="F41" s="12">
+        <v>2</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B42" s="4">
         <v>42770</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="7">
         <v>27.5</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="7">
         <v>5.3</v>
       </c>
-      <c r="F42" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="F42" s="12">
+        <v>1</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="4">
         <v>42770</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="7">
         <v>38.5</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="7">
         <v>7.1</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="12">
+        <v>2</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H43" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B44" s="4">
         <v>42770</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="7">
         <v>34.1</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="7">
         <v>7.8</v>
       </c>
-      <c r="F44" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="F44" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B45" s="4">
         <v>42770</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="7">
         <v>39.6</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="7">
         <v>7.1</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="F45" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B46" s="4">
         <v>42770</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="7">
         <v>29</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="7">
         <v>5.6</v>
       </c>
-      <c r="F46" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="F46" s="12">
+        <v>1</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B47" s="4">
         <v>42770</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="7">
         <v>38.4</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="7">
         <v>10.4</v>
       </c>
-      <c r="F47" s="8"/>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="F47" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B48" s="4">
         <v>42770</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="7">
         <v>38.4</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="7">
         <v>7.6</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F48" s="8"/>
+      <c r="F48" s="12"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
@@ -1750,13 +1823,13 @@
       <c r="B49" s="4">
         <v>42770</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="7">
         <v>25.1</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="7">
         <v>2.9</v>
       </c>
-      <c r="F49" s="8"/>
+      <c r="F49" s="12"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
@@ -1765,13 +1838,13 @@
       <c r="B50" s="4">
         <v>42770</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="7">
         <v>36.5</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="7">
         <v>8.5</v>
       </c>
-      <c r="F50" s="8"/>
+      <c r="F50" s="12"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
@@ -1780,13 +1853,13 @@
       <c r="B51" s="4">
         <v>42770</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="7">
         <v>24.5</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="7">
         <v>3.3</v>
       </c>
-      <c r="F51" s="8"/>
+      <c r="F51" s="12"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
@@ -1795,13 +1868,13 @@
       <c r="B52" s="4">
         <v>42770</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="7">
         <v>37.4</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="7">
         <v>8.4</v>
       </c>
-      <c r="F52" s="8"/>
+      <c r="F52" s="12"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
@@ -1810,13 +1883,13 @@
       <c r="B53" s="4">
         <v>42770</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="7">
         <v>40.020000000000003</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D53" s="7">
         <v>9.1</v>
       </c>
-      <c r="F53" s="8"/>
+      <c r="F53" s="12"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
@@ -1825,24 +1898,24 @@
       <c r="B54" s="4">
         <v>42770</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C54" s="7">
         <v>28.4</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="7">
         <v>5.9</v>
       </c>
-      <c r="F54" s="8"/>
+      <c r="F54" s="12"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
+        <v>133</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
       <c r="E56" s="3" t="s">
         <v>120</v>
       </c>
@@ -1854,13 +1927,13 @@
       <c r="B57" s="4">
         <v>42770</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="7">
         <v>30.56</v>
       </c>
-      <c r="D57" s="10">
+      <c r="D57" s="7">
         <v>5.7</v>
       </c>
-      <c r="F57" s="8"/>
+      <c r="F57" s="12"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
@@ -1869,13 +1942,13 @@
       <c r="B58" s="4">
         <v>42770</v>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="7">
         <v>33.5</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="7">
         <v>8.4</v>
       </c>
-      <c r="F58" s="8"/>
+      <c r="F58" s="12"/>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2" t="s">
@@ -1884,13 +1957,13 @@
       <c r="B59" s="4">
         <v>42770</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C59" s="7">
         <v>25.6</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="7">
         <v>3.5</v>
       </c>
-      <c r="F59" s="8"/>
+      <c r="F59" s="12"/>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
@@ -1899,16 +1972,16 @@
       <c r="B60" s="4">
         <v>42770</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C60" s="7">
         <v>33.4</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D60" s="7">
         <v>8.6</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F60" s="8"/>
+      <c r="F60" s="12"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
@@ -1917,16 +1990,16 @@
       <c r="B61" s="4">
         <v>42770</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C61" s="7">
         <v>36.4</v>
       </c>
-      <c r="D61" s="10">
+      <c r="D61" s="7">
         <v>9.5</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F61" s="8"/>
+      <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
@@ -1935,16 +2008,16 @@
       <c r="B62" s="4">
         <v>42770</v>
       </c>
-      <c r="C62" s="10">
+      <c r="C62" s="7">
         <v>35.5</v>
       </c>
-      <c r="D62" s="10">
+      <c r="D62" s="7">
         <v>8.6</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F62" s="8"/>
+      <c r="F62" s="12"/>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
@@ -1953,16 +2026,16 @@
       <c r="B63" s="4">
         <v>42770</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="7">
         <v>42.2</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="7">
         <v>8.6999999999999993</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F63" s="8"/>
+      <c r="F63" s="12"/>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
@@ -1971,16 +2044,16 @@
       <c r="B64" s="4">
         <v>42770</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C64" s="7">
         <v>22</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="7">
         <v>3.4</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F64" s="8"/>
+      <c r="F64" s="12"/>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
@@ -1989,16 +2062,16 @@
       <c r="B65" s="4">
         <v>42770</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="7">
         <v>35.299999999999997</v>
       </c>
-      <c r="D65" s="10">
+      <c r="D65" s="7">
         <v>5.2</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F65" s="8"/>
+      <c r="F65" s="12"/>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
@@ -2007,13 +2080,13 @@
       <c r="B66" s="4">
         <v>42770</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="7">
         <v>34.1</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="7">
         <v>5.6</v>
       </c>
-      <c r="F66" s="8"/>
+      <c r="F66" s="12"/>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
@@ -2022,13 +2095,13 @@
       <c r="B67" s="4">
         <v>42770</v>
       </c>
-      <c r="C67" s="10">
+      <c r="C67" s="7">
         <v>25.4</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D67" s="7">
         <v>4.2</v>
       </c>
-      <c r="F67" s="8"/>
+      <c r="F67" s="12"/>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
@@ -2037,16 +2110,16 @@
       <c r="B68" s="4">
         <v>42770</v>
       </c>
-      <c r="C68" s="10">
+      <c r="C68" s="7">
         <v>30.5</v>
       </c>
-      <c r="D68" s="10">
+      <c r="D68" s="7">
         <v>9.4</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F68" s="8"/>
+      <c r="F68" s="12"/>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
@@ -2055,13 +2128,13 @@
       <c r="B69" s="4">
         <v>42770</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="7">
         <v>37.119999999999997</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="7">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F69" s="8"/>
+      <c r="F69" s="12"/>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
@@ -2070,13 +2143,13 @@
       <c r="B70" s="4">
         <v>42770</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="7">
         <v>37.1</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D70" s="7">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F70" s="8"/>
+      <c r="F70" s="12"/>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2" t="s">
@@ -2085,23 +2158,23 @@
       <c r="B71" s="4">
         <v>42770</v>
       </c>
-      <c r="C71" s="10">
+      <c r="C71" s="7">
         <v>29</v>
       </c>
-      <c r="D71" s="10">
+      <c r="D71" s="7">
         <v>5.4</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
       <c r="E73" s="3" t="s">
         <v>116</v>
       </c>
@@ -2113,10 +2186,10 @@
       <c r="B74" s="4">
         <v>42770</v>
       </c>
-      <c r="C74" s="10">
+      <c r="C74" s="7">
         <v>26.1</v>
       </c>
-      <c r="D74" s="10">
+      <c r="D74" s="7">
         <v>6.7</v>
       </c>
       <c r="E74" s="3" t="s">
@@ -2130,10 +2203,10 @@
       <c r="B75" s="4">
         <v>42770</v>
       </c>
-      <c r="C75" s="10">
+      <c r="C75" s="7">
         <v>21.7</v>
       </c>
-      <c r="D75" s="10">
+      <c r="D75" s="7">
         <v>2</v>
       </c>
       <c r="E75" s="3" t="s">
@@ -2147,10 +2220,10 @@
       <c r="B76" s="4">
         <v>42770</v>
       </c>
-      <c r="C76" s="10">
+      <c r="C76" s="7">
         <v>20.3</v>
       </c>
-      <c r="D76" s="10">
+      <c r="D76" s="7">
         <v>2.6</v>
       </c>
     </row>
@@ -2161,10 +2234,10 @@
       <c r="B77" s="4">
         <v>42770</v>
       </c>
-      <c r="C77" s="10">
+      <c r="C77" s="7">
         <v>25.6</v>
       </c>
-      <c r="D77" s="10">
+      <c r="D77" s="7">
         <v>3.2</v>
       </c>
     </row>
@@ -2175,10 +2248,10 @@
       <c r="B78" s="4">
         <v>42770</v>
       </c>
-      <c r="C78" s="10">
+      <c r="C78" s="7">
         <v>30.4</v>
       </c>
-      <c r="D78" s="10">
+      <c r="D78" s="7">
         <v>4.3</v>
       </c>
     </row>
@@ -2189,10 +2262,10 @@
       <c r="B79" s="4">
         <v>42770</v>
       </c>
-      <c r="C79" s="10">
+      <c r="C79" s="7">
         <v>36.5</v>
       </c>
-      <c r="D79" s="10">
+      <c r="D79" s="7">
         <v>8.6</v>
       </c>
     </row>
@@ -2203,10 +2276,10 @@
       <c r="B80" s="4">
         <v>42770</v>
       </c>
-      <c r="C80" s="10">
+      <c r="C80" s="7">
         <v>28.9</v>
       </c>
-      <c r="D80" s="10">
+      <c r="D80" s="7">
         <v>4.7</v>
       </c>
     </row>
@@ -2217,10 +2290,10 @@
       <c r="B81" s="4">
         <v>42770</v>
       </c>
-      <c r="C81" s="10">
+      <c r="C81" s="7">
         <v>29.5</v>
       </c>
-      <c r="D81" s="10">
+      <c r="D81" s="7">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -2231,23 +2304,23 @@
       <c r="B82" s="4">
         <v>42770</v>
       </c>
-      <c r="C82" s="10">
+      <c r="C82" s="7">
         <v>35</v>
       </c>
-      <c r="D82" s="10">
+      <c r="D82" s="7">
         <v>6.9</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
       <c r="E84" s="3" t="s">
         <v>116</v>
       </c>
@@ -2259,10 +2332,10 @@
       <c r="B85" s="4">
         <v>42770</v>
       </c>
-      <c r="C85" s="10">
+      <c r="C85" s="7">
         <v>27</v>
       </c>
-      <c r="D85" s="10">
+      <c r="D85" s="7">
         <v>5.8</v>
       </c>
     </row>
@@ -2273,10 +2346,10 @@
       <c r="B86" s="4">
         <v>42770</v>
       </c>
-      <c r="C86" s="10">
+      <c r="C86" s="7">
         <v>24.2</v>
       </c>
-      <c r="D86" s="10">
+      <c r="D86" s="7">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2287,10 +2360,10 @@
       <c r="B87" s="4">
         <v>42770</v>
       </c>
-      <c r="C87" s="10">
+      <c r="C87" s="7">
         <v>30.5</v>
       </c>
-      <c r="D87" s="10">
+      <c r="D87" s="7">
         <v>5.8</v>
       </c>
     </row>
@@ -2301,10 +2374,10 @@
       <c r="B88" s="4">
         <v>42770</v>
       </c>
-      <c r="C88" s="10">
+      <c r="C88" s="7">
         <v>34.9</v>
       </c>
-      <c r="D88" s="10">
+      <c r="D88" s="7">
         <v>8.5</v>
       </c>
     </row>
@@ -2315,10 +2388,10 @@
       <c r="B89" s="4">
         <v>42770</v>
       </c>
-      <c r="C89" s="10">
+      <c r="C89" s="7">
         <v>32</v>
       </c>
-      <c r="D89" s="10">
+      <c r="D89" s="7">
         <v>5.8</v>
       </c>
     </row>
@@ -2329,10 +2402,10 @@
       <c r="B90" s="4">
         <v>42770</v>
       </c>
-      <c r="C90" s="10">
+      <c r="C90" s="7">
         <v>28</v>
       </c>
-      <c r="D90" s="10">
+      <c r="D90" s="7">
         <v>3.9</v>
       </c>
     </row>
@@ -2343,10 +2416,10 @@
       <c r="B91" s="4">
         <v>42770</v>
       </c>
-      <c r="C91" s="10">
+      <c r="C91" s="7">
         <v>34.700000000000003</v>
       </c>
-      <c r="D91" s="10">
+      <c r="D91" s="7">
         <v>6.6</v>
       </c>
     </row>
@@ -2357,10 +2430,10 @@
       <c r="B92" s="4">
         <v>42770</v>
       </c>
-      <c r="C92" s="10">
+      <c r="C92" s="7">
         <v>34.1</v>
       </c>
-      <c r="D92" s="10">
+      <c r="D92" s="7">
         <v>7.2</v>
       </c>
     </row>
@@ -2371,16 +2444,16 @@
       <c r="B93" s="4">
         <v>42770</v>
       </c>
-      <c r="C93" s="10">
+      <c r="C93" s="7">
         <v>31</v>
       </c>
-      <c r="D93" s="10">
+      <c r="D93" s="7">
         <v>5.5</v>
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2" t="s">
@@ -2389,13 +2462,13 @@
       <c r="B95" s="4">
         <v>42777</v>
       </c>
-      <c r="C95" s="10">
+      <c r="C95" s="7">
         <v>20.02</v>
       </c>
-      <c r="D95" s="10">
+      <c r="D95" s="7">
         <v>1.5</v>
       </c>
-      <c r="F95" s="9">
+      <c r="F95" s="14">
         <v>1</v>
       </c>
     </row>
@@ -2406,13 +2479,13 @@
       <c r="B96" s="4">
         <v>42777</v>
       </c>
-      <c r="C96" s="10">
+      <c r="C96" s="7">
         <v>29.5</v>
       </c>
-      <c r="D96" s="10">
+      <c r="D96" s="7">
         <v>2.8</v>
       </c>
-      <c r="F96" s="9">
+      <c r="F96" s="14">
         <v>2</v>
       </c>
     </row>
@@ -2423,13 +2496,13 @@
       <c r="B97" s="4">
         <v>42777</v>
       </c>
-      <c r="C97" s="10">
+      <c r="C97" s="7">
         <v>18.3</v>
       </c>
-      <c r="D97" s="10">
+      <c r="D97" s="7">
         <v>1.6</v>
       </c>
-      <c r="F97" s="9">
+      <c r="F97" s="14">
         <v>3</v>
       </c>
     </row>
@@ -2440,13 +2513,13 @@
       <c r="B98" s="4">
         <v>42777</v>
       </c>
-      <c r="C98" s="10">
+      <c r="C98" s="7">
         <v>21.2</v>
       </c>
-      <c r="D98" s="10">
+      <c r="D98" s="7">
         <v>1.2</v>
       </c>
-      <c r="F98" s="9">
+      <c r="F98" s="14">
         <v>4</v>
       </c>
     </row>
@@ -2457,13 +2530,13 @@
       <c r="B99" s="4">
         <v>42777</v>
       </c>
-      <c r="C99" s="10">
+      <c r="C99" s="7">
         <v>24.3</v>
       </c>
-      <c r="D99" s="10">
+      <c r="D99" s="7">
         <v>2.6</v>
       </c>
-      <c r="F99" s="9">
+      <c r="F99" s="14">
         <v>5</v>
       </c>
     </row>
@@ -2474,13 +2547,13 @@
       <c r="B100" s="4">
         <v>42777</v>
       </c>
-      <c r="C100" s="10">
+      <c r="C100" s="7">
         <v>28.3</v>
       </c>
-      <c r="D100" s="10">
+      <c r="D100" s="7">
         <v>2.7</v>
       </c>
-      <c r="F100" s="9">
+      <c r="F100" s="14">
         <v>6</v>
       </c>
     </row>
@@ -2491,13 +2564,13 @@
       <c r="B101" s="4">
         <v>42777</v>
       </c>
-      <c r="C101" s="10">
+      <c r="C101" s="7">
         <v>20.04</v>
       </c>
-      <c r="D101" s="10">
+      <c r="D101" s="7">
         <v>1.2</v>
       </c>
-      <c r="F101" s="9">
+      <c r="F101" s="14">
         <v>7</v>
       </c>
     </row>
@@ -2508,13 +2581,13 @@
       <c r="B102" s="4">
         <v>42777</v>
       </c>
-      <c r="C102" s="10">
+      <c r="C102" s="7">
         <v>20.059999999999999</v>
       </c>
-      <c r="D102" s="10">
+      <c r="D102" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F102" s="9">
+      <c r="F102" s="14">
         <v>8</v>
       </c>
     </row>
@@ -2525,13 +2598,13 @@
       <c r="B103" s="4">
         <v>42777</v>
       </c>
-      <c r="C103" s="10">
+      <c r="C103" s="7">
         <v>16.8</v>
       </c>
-      <c r="D103" s="10">
+      <c r="D103" s="7">
         <v>0.6</v>
       </c>
-      <c r="F103" s="9">
+      <c r="F103" s="14">
         <v>9</v>
       </c>
     </row>
@@ -2542,13 +2615,13 @@
       <c r="B104" s="4">
         <v>42777</v>
       </c>
-      <c r="C104" s="10">
+      <c r="C104" s="7">
         <v>21.8</v>
       </c>
-      <c r="D104" s="10">
+      <c r="D104" s="7">
         <v>1.3</v>
       </c>
-      <c r="F104" s="9">
+      <c r="F104" s="14">
         <v>10</v>
       </c>
     </row>
@@ -2559,13 +2632,13 @@
       <c r="B105" s="4">
         <v>42777</v>
       </c>
-      <c r="C105" s="10">
+      <c r="C105" s="7">
         <v>23.7</v>
       </c>
-      <c r="D105" s="10">
+      <c r="D105" s="7">
         <v>1.9</v>
       </c>
-      <c r="F105" s="9">
+      <c r="F105" s="14">
         <v>11</v>
       </c>
     </row>
@@ -2576,13 +2649,13 @@
       <c r="B106" s="4">
         <v>42777</v>
       </c>
-      <c r="C106" s="10">
+      <c r="C106" s="7">
         <v>27.5</v>
       </c>
-      <c r="D106" s="10">
+      <c r="D106" s="7">
         <v>3</v>
       </c>
-      <c r="F106" s="9">
+      <c r="F106" s="14">
         <v>12</v>
       </c>
     </row>
@@ -2593,13 +2666,13 @@
       <c r="B107" s="4">
         <v>42777</v>
       </c>
-      <c r="C107" s="10">
+      <c r="C107" s="7">
         <v>21.6</v>
       </c>
-      <c r="D107" s="10">
+      <c r="D107" s="7">
         <v>1.6</v>
       </c>
-      <c r="F107" s="9">
+      <c r="F107" s="14">
         <v>13</v>
       </c>
     </row>
@@ -2610,13 +2683,13 @@
       <c r="B108" s="4">
         <v>42777</v>
       </c>
-      <c r="C108" s="10">
+      <c r="C108" s="7">
         <v>24.1</v>
       </c>
-      <c r="D108" s="10">
+      <c r="D108" s="7">
         <v>1.4</v>
       </c>
-      <c r="F108" s="9">
+      <c r="F108" s="14">
         <v>14</v>
       </c>
     </row>
@@ -2627,20 +2700,20 @@
       <c r="B109" s="4">
         <v>42777</v>
       </c>
-      <c r="C109" s="10">
+      <c r="C109" s="7">
         <v>22.5</v>
       </c>
-      <c r="D109" s="10">
+      <c r="D109" s="7">
         <v>1.5</v>
       </c>
-      <c r="F109" s="9">
+      <c r="F109" s="14">
         <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="F110" s="9" t="s">
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="F110" s="14" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2651,13 +2724,13 @@
       <c r="B111" s="4">
         <v>42777</v>
       </c>
-      <c r="C111" s="10">
+      <c r="C111" s="7">
         <v>23.8</v>
       </c>
-      <c r="D111" s="10">
+      <c r="D111" s="7">
         <v>2.1</v>
       </c>
-      <c r="F111" s="9">
+      <c r="F111" s="14">
         <v>16</v>
       </c>
     </row>
@@ -2668,13 +2741,13 @@
       <c r="B112" s="4">
         <v>42777</v>
       </c>
-      <c r="C112" s="10">
+      <c r="C112" s="7">
         <v>21.5</v>
       </c>
-      <c r="D112" s="10">
+      <c r="D112" s="7">
         <v>1.8</v>
       </c>
-      <c r="F112" s="9">
+      <c r="F112" s="14">
         <v>17</v>
       </c>
     </row>
@@ -2685,13 +2758,13 @@
       <c r="B113" s="4">
         <v>42777</v>
       </c>
-      <c r="C113" s="10">
+      <c r="C113" s="7">
         <v>24.6</v>
       </c>
-      <c r="D113" s="10">
+      <c r="D113" s="7">
         <v>2.6</v>
       </c>
-      <c r="F113" s="9">
+      <c r="F113" s="14">
         <v>18</v>
       </c>
     </row>
@@ -2702,13 +2775,13 @@
       <c r="B114" s="4">
         <v>42777</v>
       </c>
-      <c r="C114" s="10">
+      <c r="C114" s="7">
         <v>17.7</v>
       </c>
-      <c r="D114" s="10">
+      <c r="D114" s="7">
         <v>1.3</v>
       </c>
-      <c r="F114" s="9">
+      <c r="F114" s="14">
         <v>19</v>
       </c>
     </row>
@@ -2719,13 +2792,13 @@
       <c r="B115" s="4">
         <v>42777</v>
       </c>
-      <c r="C115" s="10">
+      <c r="C115" s="7">
         <v>16.899999999999999</v>
       </c>
-      <c r="D115" s="10">
+      <c r="D115" s="7">
         <v>0.6</v>
       </c>
-      <c r="F115" s="9">
+      <c r="F115" s="14">
         <v>20</v>
       </c>
     </row>
@@ -2736,13 +2809,13 @@
       <c r="B116" s="4">
         <v>42777</v>
       </c>
-      <c r="C116" s="10">
+      <c r="C116" s="7">
         <v>19.5</v>
       </c>
-      <c r="D116" s="10">
+      <c r="D116" s="7">
         <v>1</v>
       </c>
-      <c r="F116" s="9">
+      <c r="F116" s="14">
         <v>21</v>
       </c>
     </row>
@@ -2753,13 +2826,13 @@
       <c r="B117" s="4">
         <v>42777</v>
       </c>
-      <c r="C117" s="10">
+      <c r="C117" s="7">
         <v>19.899999999999999</v>
       </c>
-      <c r="D117" s="10">
+      <c r="D117" s="7">
         <v>1.6</v>
       </c>
-      <c r="F117" s="9">
+      <c r="F117" s="14">
         <v>22</v>
       </c>
     </row>
@@ -2770,13 +2843,13 @@
       <c r="B118" s="4">
         <v>42777</v>
       </c>
-      <c r="C118" s="10">
+      <c r="C118" s="7">
         <v>19.5</v>
       </c>
-      <c r="D118" s="10">
+      <c r="D118" s="7">
         <v>1.5</v>
       </c>
-      <c r="F118" s="9">
+      <c r="F118" s="14">
         <v>23</v>
       </c>
     </row>
@@ -2787,13 +2860,13 @@
       <c r="B119" s="4">
         <v>42777</v>
       </c>
-      <c r="C119" s="10">
+      <c r="C119" s="7">
         <v>21.5</v>
       </c>
-      <c r="D119" s="10">
+      <c r="D119" s="7">
         <v>1.3</v>
       </c>
-      <c r="F119" s="9">
+      <c r="F119" s="14">
         <v>24</v>
       </c>
     </row>
@@ -2804,13 +2877,13 @@
       <c r="B120" s="4">
         <v>42777</v>
       </c>
-      <c r="C120" s="10">
+      <c r="C120" s="7">
         <v>22.5</v>
       </c>
-      <c r="D120" s="10">
+      <c r="D120" s="7">
         <v>1.9</v>
       </c>
-      <c r="F120" s="9">
+      <c r="F120" s="14">
         <v>25</v>
       </c>
     </row>
@@ -2821,13 +2894,13 @@
       <c r="B121" s="4">
         <v>42777</v>
       </c>
-      <c r="C121" s="10">
+      <c r="C121" s="7">
         <v>18.7</v>
       </c>
-      <c r="D121" s="10">
+      <c r="D121" s="7">
         <v>1.2</v>
       </c>
-      <c r="F121" s="9">
+      <c r="F121" s="14">
         <v>26</v>
       </c>
     </row>
@@ -2838,13 +2911,13 @@
       <c r="B122" s="4">
         <v>42777</v>
       </c>
-      <c r="C122" s="10">
+      <c r="C122" s="7">
         <v>18.600000000000001</v>
       </c>
-      <c r="D122" s="10">
+      <c r="D122" s="7">
         <v>1.3</v>
       </c>
-      <c r="F122" s="9">
+      <c r="F122" s="14">
         <v>27</v>
       </c>
     </row>
@@ -2855,13 +2928,13 @@
       <c r="B123" s="4">
         <v>42777</v>
       </c>
-      <c r="C123" s="10">
+      <c r="C123" s="7">
         <v>26.5</v>
       </c>
-      <c r="D123" s="10">
+      <c r="D123" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F123" s="9">
+      <c r="F123" s="14">
         <v>28</v>
       </c>
     </row>
@@ -2872,13 +2945,13 @@
       <c r="B124" s="4">
         <v>42777</v>
       </c>
-      <c r="C124" s="10">
+      <c r="C124" s="7">
         <v>25</v>
       </c>
-      <c r="D124" s="10">
+      <c r="D124" s="7">
         <v>1.9</v>
       </c>
-      <c r="F124" s="9">
+      <c r="F124" s="14">
         <v>29</v>
       </c>
     </row>
@@ -2889,13 +2962,13 @@
       <c r="B125" s="4">
         <v>42777</v>
       </c>
-      <c r="C125" s="10">
+      <c r="C125" s="7">
         <v>21.3</v>
       </c>
-      <c r="D125" s="10">
+      <c r="D125" s="7">
         <v>1.3</v>
       </c>
-      <c r="F125" s="9">
+      <c r="F125" s="14">
         <v>30</v>
       </c>
     </row>

</xml_diff>